<commit_message>
Se crean archivos con funciones genéricas para el consumo del webservice por módulo.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
+++ b/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_portal\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DF4952-26C7-46AB-8E3E-05AAAC17640E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7503E1D-1437-4BBD-B8C0-2850BF015207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Finanzas</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>resumen_lotes_can.asp</t>
+  </si>
+  <si>
+    <t>Enrique</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A1D6-7B71-47BA-AFC3-09F2C41CC057}">
   <dimension ref="A2:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1145,9 @@
       <c r="G14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="I14" s="14" t="s">
         <v>56</v>
       </c>
@@ -1282,8 +1287,12 @@
       <c r="G20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="H20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J20" s="17"/>
       <c r="K20" s="17"/>
       <c r="M20" s="4"/>
@@ -1306,8 +1315,12 @@
       <c r="G21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="H21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J21" s="17"/>
       <c r="K21" s="17"/>
       <c r="M21" s="4"/>

</xml_diff>

<commit_message>
Se actualiza plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
+++ b/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_portal\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7503E1D-1437-4BBD-B8C0-2850BF015207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D41B0E-07D3-494C-8A89-BA13294D3461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
   <si>
     <t>Finanzas</t>
   </si>
@@ -277,13 +277,25 @@
   </si>
   <si>
     <t>Enrique</t>
+  </si>
+  <si>
+    <t>Descargar talones (txt)</t>
+  </si>
+  <si>
+    <t>Imprimir etiquetas</t>
+  </si>
+  <si>
+    <t>ltl_consulta-dl.asp?tipo=txt</t>
+  </si>
+  <si>
+    <t>print_label.asp?nui=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -336,13 +348,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -363,10 +387,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -426,8 +451,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -745,10 +777,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A1D6-7B71-47BA-AFC3-09F2C41CC057}">
-  <dimension ref="A2:Q25"/>
+  <dimension ref="A2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +918,7 @@
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="21" t="s">
         <v>15</v>
       </c>
       <c r="G5" s="14" t="s">
@@ -915,7 +949,7 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -958,8 +992,12 @@
       <c r="G7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
+      <c r="H7" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
       <c r="L7" s="11" t="s">
@@ -974,57 +1012,59 @@
       <c r="Q7" s="14"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="4"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="8" t="s">
-        <v>18</v>
+        <v>80</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
+        <v>82</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>75</v>
-      </c>
+      <c r="L8" s="11"/>
+      <c r="M8" s="20"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>5</v>
+      <c r="A9" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="11" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -1033,146 +1073,154 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-    </row>
-    <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J11" s="14"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>78</v>
-      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="20"/>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="8" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>68</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="G15" s="14"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -1184,21 +1232,25 @@
       <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>11</v>
+      <c r="A16" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="F16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="M16" s="4"/>
@@ -1207,60 +1259,72 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="8" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -1274,77 +1338,69 @@
       <c r="Q19" s="3"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
+      <c r="A20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
+      <c r="A22" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="9" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+        <v>59</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="M22" s="4"/>
@@ -1355,20 +1411,24 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
       <c r="F23" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+        <v>60</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="J23" s="17"/>
       <c r="K23" s="17"/>
       <c r="M23" s="4"/>
@@ -1377,47 +1437,95 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="8" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+    </row>
+    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G26" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="8" t="s">
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="19" t="s">
+      <c r="G27" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="3"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se actualiza cuadro de módulos y archivos considerados en la migración del portal web
</commit_message>
<xml_diff>
--- a/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
+++ b/00-Documentacion/Modulos_Portal-Asignaciones - v001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_portal\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D41B0E-07D3-494C-8A89-BA13294D3461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7243719-7BD5-4309-A82D-ADBAEBD8A72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F6A2EFE-E3EB-4DC2-84D3-28EF1475911D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>Finanzas</t>
   </si>
@@ -289,13 +289,95 @@
   </si>
   <si>
     <t>print_label.asp?nui=</t>
+  </si>
+  <si>
+    <t>state-account.asp
+state-det.asp
+state-det-dl.asp
+validaoperacion.asp
+invoice-det.asp
+Folio-Resumen.asp
+FolioAir.asp
+FolioMar.asp
+FolioTer.asp
+invoice-print.asp
+xml_factura.asp
+ltl_invoice-det-dl.asp
+Adv-Rec-Pay.asp
+supp-det.asp
+foliod-entry.asp
+anx24-dl.asp
+dict-fisc-dl.asp
+folio-dl.asp
+photos_view.asp
+download_file.asp
+det-chq.asp
+supp-det-dl.asp
+dl-operation.asp
+dl-mail.asp
+supp-det-dl2.asp</t>
+  </si>
+  <si>
+    <t>invoice-search.asp?inv_type=a
+invoices.asp
+invoices-dl.asp</t>
+  </si>
+  <si>
+    <t>invoice-search.asp?inv_type=a&amp;inv_mode=f
+invoices.asp
+invoices-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I01
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I01&amp;mode=LPR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I01&amp;mode=PR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I02&amp;mode=PR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I02&amp;mode=LPR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?concept=I02
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?mode=PR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp?mode=LPR
+payments.asp
+payments-dl.asp</t>
+  </si>
+  <si>
+    <t>payment-search.asp
+payments.asp
+payments-dl.asp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +437,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -391,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -456,6 +544,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -777,107 +868,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED06A1D6-7B71-47BA-AFC3-09F2C41CC057}">
-  <dimension ref="A2:Q27"/>
+  <dimension ref="A2:R27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="35.140625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="42.42578125" customWidth="1"/>
-    <col min="14" max="17" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="42.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
+    <col min="9" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="35.140625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="42.42578125" customWidth="1"/>
+    <col min="15" max="18" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="L2" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="N2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="O2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="P2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="P2" s="15" t="s">
+      <c r="Q2" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="15" t="s">
+      <c r="R2" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="375" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16"/>
+      <c r="B3" s="18" t="s">
+        <v>84</v>
+      </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="16"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="16"/>
+      <c r="M3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="N3" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="N3" s="16"/>
       <c r="O3" s="16"/>
       <c r="P3" s="16"/>
       <c r="Q3" s="16"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -885,649 +983,696 @@
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="K4" s="14"/>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="14"/>
+      <c r="M4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="N4" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="N4" s="14"/>
       <c r="O4" s="14"/>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="14"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="12" t="s">
+      <c r="L5" s="14"/>
+      <c r="M5" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="14"/>
       <c r="N5" s="14"/>
       <c r="O5" s="14"/>
       <c r="P5" s="14"/>
       <c r="Q5" s="14"/>
-    </row>
-    <row r="6" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="14"/>
+      <c r="B6" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="14"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="18" t="s">
+      <c r="N6" s="18" t="s">
         <v>53</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="O6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="P6" s="14"/>
+      <c r="P6" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="Q6" s="14"/>
-    </row>
-    <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
+      <c r="B7" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="H7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J7" s="14"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="11" t="s">
+      <c r="L7" s="14"/>
+      <c r="M7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="N7" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="H8" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="J8" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="14"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="20"/>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="14"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>85</v>
+      </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="H9" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="I9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="11" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="N9" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="14"/>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>86</v>
+      </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="H10" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="J10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="11" t="s">
+      <c r="L10" s="14"/>
+      <c r="M10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="N10" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="R10" s="14"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="H11" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="I11" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="J11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="14"/>
       <c r="K11" s="14"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="16"/>
+      <c r="R11" s="14"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="14"/>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="16"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="11" t="s">
+      <c r="L12" s="16"/>
+      <c r="M12" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="N12" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="N12" s="16"/>
       <c r="O12" s="16"/>
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
-    </row>
-    <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="14"/>
+      <c r="R12" s="16"/>
+    </row>
+    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="H13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
-      <c r="L13" s="11" t="s">
+      <c r="L13" s="14"/>
+      <c r="M13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="N13" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="14"/>
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>88</v>
+      </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="14"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="14"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="17"/>
+        <v>6</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="17"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
-    </row>
-    <row r="16" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="17"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="17"/>
+      <c r="G16" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="H16" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="I16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J16" s="17"/>
       <c r="K16" s="17"/>
-      <c r="M16" s="4"/>
+      <c r="L16" s="17"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
-    </row>
-    <row r="17" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="17"/>
+        <v>9</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>90</v>
+      </c>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="17"/>
+      <c r="G17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="H17" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I17" s="17" t="s">
+      <c r="J17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J17" s="17"/>
       <c r="K17" s="17"/>
-      <c r="M17" s="4"/>
+      <c r="L17" s="17"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
-    </row>
-    <row r="18" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="17"/>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="1:18" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>91</v>
+      </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="17"/>
+      <c r="G18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="I18" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I18" s="17" t="s">
+      <c r="J18" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J18" s="17"/>
       <c r="K18" s="17"/>
-      <c r="M18" s="4"/>
+      <c r="L18" s="17"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>92</v>
+      </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="M19" s="3"/>
+      <c r="L19" s="14"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>12</v>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="14"/>
+      <c r="G20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="14"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>93</v>
+      </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
-      <c r="M21" s="3"/>
+      <c r="L21" s="14"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="17"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>94</v>
+      </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="17"/>
+      <c r="G22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="H22" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="I22" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="J22" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="17"/>
       <c r="K22" s="17"/>
-      <c r="M22" s="4"/>
+      <c r="L22" s="17"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="4"/>
+    </row>
+    <row r="23" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="17"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>95</v>
+      </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
-      <c r="F23" s="9" t="s">
+      <c r="F23" s="17"/>
+      <c r="G23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="H23" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="I23" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="J23" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="J23" s="17"/>
       <c r="K23" s="17"/>
-      <c r="M23" s="4"/>
+      <c r="L23" s="17"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="17"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B24" s="14"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="H24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
       <c r="K24" s="17"/>
-      <c r="M24" s="4"/>
+      <c r="L24" s="17"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" s="17"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B25" s="14"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
-      <c r="F25" s="9" t="s">
+      <c r="F25" s="17"/>
+      <c r="G25" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="H25" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
       <c r="K25" s="17"/>
-      <c r="M25" s="4"/>
+      <c r="L25" s="17"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
-    </row>
-    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="3"/>
+      <c r="G26" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G26" s="19" t="s">
+      <c r="H26" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
       <c r="K26" s="14"/>
-      <c r="M26" s="3"/>
+      <c r="L26" s="14"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="3"/>
+      <c r="G27" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="H27" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
       <c r="K27" s="14"/>
-      <c r="M27" s="3"/>
+      <c r="L27" s="14"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>